<commit_message>
Working IEEE models and ORPD.
Remaining: Generator losses, generator reactive power constraints, stochastic consumption model.
</commit_message>
<xml_diff>
--- a/simplepower/models/grid_model_data/grid_data1.xlsx
+++ b/simplepower/models/grid_model_data/grid_data1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uisn-my.sharepoint.com/personal/emelf_usn_no/Documents/PhD - SysOpt/Python Work/Custom Modules/simplepower/simplepower/models/grid_model_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="136" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D00D4CC-D955-45D7-93DD-73BF2D4F11DC}"/>
+  <xr:revisionPtr revIDLastSave="140" documentId="8_{76AC49D0-40D7-45F9-8AB9-9B675F322E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3E64B57-52D9-4D2F-89C8-E791917AB6A5}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2010" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{120A7045-FD09-44EC-B7BA-2F1FCE4B68C8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{120A7045-FD09-44EC-B7BA-2F1FCE4B68C8}"/>
   </bookViews>
   <sheets>
     <sheet name="busbars" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>name</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>v_base_kV</t>
+  </si>
+  <si>
+    <t>I_lim_A</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F24F74-C913-4254-AF10-9102B3F26C94}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +587,7 @@
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,28 +595,31 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -621,24 +627,27 @@
         <v>22</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <v>4</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
         <v>0</v>
       </c>
     </row>
@@ -782,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F16A2ED-50B9-4F00-806A-3112A6263A70}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>